<commit_message>
Updated code for online customer creation
</commit_message>
<xml_diff>
--- a/File/customerPersonalinformation.xlsx
+++ b/File/customerPersonalinformation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="68">
   <si>
     <t xml:space="preserve">testId</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">TC_01</t>
   </si>
   <si>
-    <t xml:space="preserve">Validating the positive journey</t>
+    <t xml:space="preserve">Validating the flow with Religion “Hindu”</t>
   </si>
   <si>
     <t xml:space="preserve">Graduation</t>
@@ -86,6 +86,180 @@
   </si>
   <si>
     <t xml:space="preserve">Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Muslim ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muslim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Christan”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Sikh”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Buddhism”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buddhism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Jainism”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jainism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Parsi”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating the flow with Religion “Others”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transgender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_16</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">12</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Graduation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Formal Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional Degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unmarried</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divorced</t>
   </si>
 </sst>
 </file>
@@ -95,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +290,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,13 +367,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
   </cols>
@@ -252,7 +433,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>3345768571</v>
+        <v>3898738743</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>16</v>
@@ -272,6 +453,769 @@
       <c r="L2" s="0" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>3898738743</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>3898738744</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>3898738745</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>3898738746</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>3898738747</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>3898738748</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>3898738749</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3898738750</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>3898738751</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3898738752</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>3898738753</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>3898738754</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K23" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>